<commit_message>
Reform of the correct structure for the seed.js
</commit_message>
<xml_diff>
--- a/src/assets/files/personal.xlsx
+++ b/src/assets/files/personal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19830" windowHeight="9120"/>
+    <workbookView windowWidth="20775" windowHeight="10155"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3918" uniqueCount="2252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4497" uniqueCount="2588">
   <si>
     <t>AEROPUERTO ALBERTO CARNEVALLI - MERIDA</t>
   </si>
@@ -6770,6 +6770,1014 @@
   </si>
   <si>
     <t>WILLIAMS RAMON</t>
+  </si>
+  <si>
+    <t>BAER SEDE CENTRAL</t>
+  </si>
+  <si>
+    <t>VALERO RIVAS</t>
+  </si>
+  <si>
+    <t>YELITZA CAROLINA</t>
+  </si>
+  <si>
+    <t>BARRIOS</t>
+  </si>
+  <si>
+    <t>PEDRO VICENTE</t>
+  </si>
+  <si>
+    <t>EVA ISMELIA</t>
+  </si>
+  <si>
+    <t>APARICIO VINACHE</t>
+  </si>
+  <si>
+    <t>PEREZ GONZALEZ</t>
+  </si>
+  <si>
+    <t>EDWIN RAFAEL</t>
+  </si>
+  <si>
+    <t>EURRESTA MANCIPE</t>
+  </si>
+  <si>
+    <t>MANGANESE MASTROLONARDO</t>
+  </si>
+  <si>
+    <t>ENRICO</t>
+  </si>
+  <si>
+    <t>PERAZA CAMEJO</t>
+  </si>
+  <si>
+    <t>RAMON FLORES</t>
+  </si>
+  <si>
+    <t>BLANCO TORREALBA</t>
+  </si>
+  <si>
+    <t>EMMA INOCENCIA</t>
+  </si>
+  <si>
+    <t>HERRERA ALVARADO</t>
+  </si>
+  <si>
+    <t>LILA DEL CARMEN</t>
+  </si>
+  <si>
+    <t>ARCILES TORO</t>
+  </si>
+  <si>
+    <t>YURELIS SCARLET</t>
+  </si>
+  <si>
+    <t>AVENDAÑO CHAVEZ</t>
+  </si>
+  <si>
+    <t>JACQUELINE MARIA</t>
+  </si>
+  <si>
+    <t>VELASQUEZ LEON</t>
+  </si>
+  <si>
+    <t>ESTRADA ZARRAGA</t>
+  </si>
+  <si>
+    <t>DURBETTY JOSEFINA</t>
+  </si>
+  <si>
+    <t>FRANCYS ZULEYMA</t>
+  </si>
+  <si>
+    <t>AVILCAR JOSE</t>
+  </si>
+  <si>
+    <t>REYES DE HERNANDEZ</t>
+  </si>
+  <si>
+    <t>DALINME</t>
+  </si>
+  <si>
+    <t>PACHECO MARTINEZ</t>
+  </si>
+  <si>
+    <t>HERNAN ENRIQUE</t>
+  </si>
+  <si>
+    <t>HERRERA BORGES</t>
+  </si>
+  <si>
+    <t>MARILYN</t>
+  </si>
+  <si>
+    <t>SANCHEZ THIELEN</t>
+  </si>
+  <si>
+    <t>RODOLFO JESUS</t>
+  </si>
+  <si>
+    <t>DUQUE RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>YORSIDE JENNIFER</t>
+  </si>
+  <si>
+    <t>ROMERO RAMOS</t>
+  </si>
+  <si>
+    <t>MARIA EUGENIA</t>
+  </si>
+  <si>
+    <t>MANZANO ANDRADE</t>
+  </si>
+  <si>
+    <t>JONATHAN</t>
+  </si>
+  <si>
+    <t>MARRERO GOMEZ</t>
+  </si>
+  <si>
+    <t>RUTH DOLORES</t>
+  </si>
+  <si>
+    <t>DIAZ HADDAD</t>
+  </si>
+  <si>
+    <t>ESCOBAR SCOTT</t>
+  </si>
+  <si>
+    <t>IRIS YELITZA</t>
+  </si>
+  <si>
+    <t>COLMENARES MARTINEZ</t>
+  </si>
+  <si>
+    <t>VICENTE PAUL</t>
+  </si>
+  <si>
+    <t>MEDINA SANCHEZ</t>
+  </si>
+  <si>
+    <t>AQUILES ALEXANDER</t>
+  </si>
+  <si>
+    <t>GIL CASTELLANO</t>
+  </si>
+  <si>
+    <t>CLEVER AZAEL</t>
+  </si>
+  <si>
+    <t>CEDRES UMANES</t>
+  </si>
+  <si>
+    <t>JOSE BUCHANAN</t>
+  </si>
+  <si>
+    <t>ALVARADO NAVARRO</t>
+  </si>
+  <si>
+    <t>HILDALIS JOSEFINA</t>
+  </si>
+  <si>
+    <t>HERRERA RAMIREZ</t>
+  </si>
+  <si>
+    <t>LILIBETH</t>
+  </si>
+  <si>
+    <t>MUJICA MENESES</t>
+  </si>
+  <si>
+    <t>ANDERSON</t>
+  </si>
+  <si>
+    <t>CORTEZ TORRES</t>
+  </si>
+  <si>
+    <t>YELITZA ISABEL</t>
+  </si>
+  <si>
+    <t>COBOS QUINTANA</t>
+  </si>
+  <si>
+    <t>CRISTOBAL RAFAEL</t>
+  </si>
+  <si>
+    <t>RONDON LINERO</t>
+  </si>
+  <si>
+    <t>ROSELING YUSVEL</t>
+  </si>
+  <si>
+    <t>BRICEÑO DUDAMEL</t>
+  </si>
+  <si>
+    <t>LEONARDO ALBERTO</t>
+  </si>
+  <si>
+    <t>FIGUEROA OBISPO</t>
+  </si>
+  <si>
+    <t>KATIUSKA JOSE</t>
+  </si>
+  <si>
+    <t>PALACIOS OROPEZA</t>
+  </si>
+  <si>
+    <t>NELYIS MARGARITA</t>
+  </si>
+  <si>
+    <t>PEREZ MAVO</t>
+  </si>
+  <si>
+    <t>DANIEL AUGUSTO</t>
+  </si>
+  <si>
+    <t>ESPINOZA GARNIER</t>
+  </si>
+  <si>
+    <t>RICHARD ALFONSO</t>
+  </si>
+  <si>
+    <t>GOMEZ DE GONZALEZ</t>
+  </si>
+  <si>
+    <t>JOHANA MARIA</t>
+  </si>
+  <si>
+    <t>LOVERA SOLORZANO</t>
+  </si>
+  <si>
+    <t>FELIX JAVIER</t>
+  </si>
+  <si>
+    <t>LISCANO BRACHO</t>
+  </si>
+  <si>
+    <t>JOSÉ ALBERTO</t>
+  </si>
+  <si>
+    <t>PEÑA CAMPOS</t>
+  </si>
+  <si>
+    <t>AUGUSTO CESAR</t>
+  </si>
+  <si>
+    <t>MOSQUERA ARIAS</t>
+  </si>
+  <si>
+    <t>PATRICIA</t>
+  </si>
+  <si>
+    <t>GUARINO LEON</t>
+  </si>
+  <si>
+    <t>ANGGY LISET</t>
+  </si>
+  <si>
+    <t>LEYRA MERCEDES</t>
+  </si>
+  <si>
+    <t>LOREYLIS DANIELA</t>
+  </si>
+  <si>
+    <t>HERNANDEZ QUINTERO</t>
+  </si>
+  <si>
+    <t>VELASQUEZ BONILLA</t>
+  </si>
+  <si>
+    <t>AURA VIOLETA</t>
+  </si>
+  <si>
+    <t>GELIMICH REYES</t>
+  </si>
+  <si>
+    <t>ROXANA JUDITH</t>
+  </si>
+  <si>
+    <t>PINTO AGUILAR</t>
+  </si>
+  <si>
+    <t>MAZA PALACIOS</t>
+  </si>
+  <si>
+    <t>ANAIS DEL VALLE</t>
+  </si>
+  <si>
+    <t>BERNAL MORALES</t>
+  </si>
+  <si>
+    <t>DEIDRE ANTONIETA</t>
+  </si>
+  <si>
+    <t>FLORES GOITIA</t>
+  </si>
+  <si>
+    <t>COREIMA MINERVI</t>
+  </si>
+  <si>
+    <t>PARRA ROCHE</t>
+  </si>
+  <si>
+    <t>DANIA MARGARITA</t>
+  </si>
+  <si>
+    <t>FLORES TOVAR</t>
+  </si>
+  <si>
+    <t>ILIANA JOSE</t>
+  </si>
+  <si>
+    <t>CASTELLON BANQUEZ</t>
+  </si>
+  <si>
+    <t>CALDERON SALAZAR</t>
+  </si>
+  <si>
+    <t>JENNY CAROLINA</t>
+  </si>
+  <si>
+    <t>CORDERO DELGADO</t>
+  </si>
+  <si>
+    <t>DORIS MIRIAM</t>
+  </si>
+  <si>
+    <t>GIMENEZ QUINTERO</t>
+  </si>
+  <si>
+    <t>YAJAIRA DEL CARMEN</t>
+  </si>
+  <si>
+    <t>BERRIO JULIO</t>
+  </si>
+  <si>
+    <t>INGRID JOHANA</t>
+  </si>
+  <si>
+    <t>LEON MARCANO</t>
+  </si>
+  <si>
+    <t>CARLOS MIGUEL</t>
+  </si>
+  <si>
+    <t>BARRIOS NUÑEZ</t>
+  </si>
+  <si>
+    <t>CASTILLO CAMEJO</t>
+  </si>
+  <si>
+    <t>YERLIN</t>
+  </si>
+  <si>
+    <t>MEDINA CORDONES</t>
+  </si>
+  <si>
+    <t>ELINEFFER NATALY</t>
+  </si>
+  <si>
+    <t>PARRA ANGULO</t>
+  </si>
+  <si>
+    <t>PASTORA DE LA CHICHINQUIRA</t>
+  </si>
+  <si>
+    <t>RUBI OROPEZA</t>
+  </si>
+  <si>
+    <t>YEIKOR ENRIQUE</t>
+  </si>
+  <si>
+    <t>AGUILERA SOTILLO</t>
+  </si>
+  <si>
+    <t>EDWARD ROBERTO</t>
+  </si>
+  <si>
+    <t>GONZALEZ ALVAREZ</t>
+  </si>
+  <si>
+    <t>PEDRO ISMAEL</t>
+  </si>
+  <si>
+    <t>ROJAS BERROTERAN</t>
+  </si>
+  <si>
+    <t>MIRAIDA MARIA</t>
+  </si>
+  <si>
+    <t>WINDER JOSE</t>
+  </si>
+  <si>
+    <t>FERNANDEZ SALAZAR</t>
+  </si>
+  <si>
+    <t>SERYIS JOSE</t>
+  </si>
+  <si>
+    <t>AGREDA SIRA</t>
+  </si>
+  <si>
+    <t>MEDINA DE VERASTEGUI</t>
+  </si>
+  <si>
+    <t>JERINYER MARSIRE</t>
+  </si>
+  <si>
+    <t>ALVAREZ DELGADO</t>
+  </si>
+  <si>
+    <t>SANDRA PATRICIA DEL VALLE</t>
+  </si>
+  <si>
+    <t>GRATEROL BORRAJO</t>
+  </si>
+  <si>
+    <t>JULIO ALFREDO</t>
+  </si>
+  <si>
+    <t>LIENDO GALVIS</t>
+  </si>
+  <si>
+    <t>ANA CECILIA</t>
+  </si>
+  <si>
+    <t>COFFI RIERA</t>
+  </si>
+  <si>
+    <t>NELSON LEONARDO</t>
+  </si>
+  <si>
+    <t>ORDOSGOITTI VILLEGAS</t>
+  </si>
+  <si>
+    <t>KEMBERLING AILICEC</t>
+  </si>
+  <si>
+    <t>RIVERA TINEO</t>
+  </si>
+  <si>
+    <t>ANA KARINA</t>
+  </si>
+  <si>
+    <t>GONZALEZ PEÑA</t>
+  </si>
+  <si>
+    <t>JESSAMYN LARIRET</t>
+  </si>
+  <si>
+    <t>MUÑOZ</t>
+  </si>
+  <si>
+    <t>LIANA CAROLINA</t>
+  </si>
+  <si>
+    <t>RUIZ PEREZ</t>
+  </si>
+  <si>
+    <t>JESUS FRANCISCO</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ MENDEZ</t>
+  </si>
+  <si>
+    <t>JOAN RENE</t>
+  </si>
+  <si>
+    <t>QUINTANA GUEDEZ</t>
+  </si>
+  <si>
+    <t>MAILIW AIXA</t>
+  </si>
+  <si>
+    <t>OLIVARES HURTADO</t>
+  </si>
+  <si>
+    <t>GABRIELA EMPERATRIZ</t>
+  </si>
+  <si>
+    <t>CASTRO PACHECO</t>
+  </si>
+  <si>
+    <t>JEAN ALBERTO</t>
+  </si>
+  <si>
+    <t>FLORES</t>
+  </si>
+  <si>
+    <t>MARIA FERNANDA</t>
+  </si>
+  <si>
+    <t>ROMERO MEJIAS</t>
+  </si>
+  <si>
+    <t>YARIZ CRISTINA</t>
+  </si>
+  <si>
+    <t>SUAREZ GOMEZ</t>
+  </si>
+  <si>
+    <t>NATHALIA BELEN</t>
+  </si>
+  <si>
+    <t>CASTRO</t>
+  </si>
+  <si>
+    <t>YIGETH SARAI</t>
+  </si>
+  <si>
+    <t>VILORIA M</t>
+  </si>
+  <si>
+    <t>DESIREE A</t>
+  </si>
+  <si>
+    <t>PINO PALACIOS</t>
+  </si>
+  <si>
+    <t>DONYI MANUEL</t>
+  </si>
+  <si>
+    <t>DIAZ BARRIOS</t>
+  </si>
+  <si>
+    <t>DAYANA LITZAY</t>
+  </si>
+  <si>
+    <t>RIVAS SANDOVAL</t>
+  </si>
+  <si>
+    <t>CARLA VANESKA</t>
+  </si>
+  <si>
+    <t>ECHEZURIA PEÑALOZA</t>
+  </si>
+  <si>
+    <t>YHAM MARCO</t>
+  </si>
+  <si>
+    <t>AVILIO JOSE</t>
+  </si>
+  <si>
+    <t>CARDONA SANCHEZ</t>
+  </si>
+  <si>
+    <t>TOVAR CASTELLANO</t>
+  </si>
+  <si>
+    <t>ELIVER JOSE</t>
+  </si>
+  <si>
+    <t>OLLARVES TORIN</t>
+  </si>
+  <si>
+    <t>KATHERINE YISSEL</t>
+  </si>
+  <si>
+    <t>QUINTERO GONZALEZ</t>
+  </si>
+  <si>
+    <t>KISUANLLER ROBERLI</t>
+  </si>
+  <si>
+    <t>LOPEZ SANOJA</t>
+  </si>
+  <si>
+    <t>DAMARIS SARAY</t>
+  </si>
+  <si>
+    <t>MUJICA TORRES</t>
+  </si>
+  <si>
+    <t>MARIAN ANDREINA</t>
+  </si>
+  <si>
+    <t>VARGAS OBISPO</t>
+  </si>
+  <si>
+    <t>ARMAS MACHADO</t>
+  </si>
+  <si>
+    <t>SANCHEZ UBLASI</t>
+  </si>
+  <si>
+    <t>MILAGROS YASELIN</t>
+  </si>
+  <si>
+    <t>VILCHEZ SANCHEZ</t>
+  </si>
+  <si>
+    <t>JEFFERSON RAFAEL</t>
+  </si>
+  <si>
+    <t>CORDONES YARAURE</t>
+  </si>
+  <si>
+    <t>EUCLIMAR MILAGROS</t>
+  </si>
+  <si>
+    <t>TREJO PALACIOS</t>
+  </si>
+  <si>
+    <t>YONDER ENRIQUE</t>
+  </si>
+  <si>
+    <t>VARGAS GUEVARA</t>
+  </si>
+  <si>
+    <t>ROTCEH ESTEFANIA</t>
+  </si>
+  <si>
+    <t>PERALTA CARVALLO</t>
+  </si>
+  <si>
+    <t>GAMBOA HIGUEREY</t>
+  </si>
+  <si>
+    <t>ANTHONY JOSE</t>
+  </si>
+  <si>
+    <t>BLANCO CHANGAROTE</t>
+  </si>
+  <si>
+    <t>NANYEL YUSMAN</t>
+  </si>
+  <si>
+    <t>MARCANO ROJAS</t>
+  </si>
+  <si>
+    <t>ARGENIS EMMANUEL</t>
+  </si>
+  <si>
+    <t>CALDERON SARATE</t>
+  </si>
+  <si>
+    <t>JEYMI ALEXANDRA</t>
+  </si>
+  <si>
+    <t>SEPULVEDA GARCIA</t>
+  </si>
+  <si>
+    <t>MOYA CAMPINS</t>
+  </si>
+  <si>
+    <t>ORIANNA DANIELA</t>
+  </si>
+  <si>
+    <t>PIRE MENDOZA</t>
+  </si>
+  <si>
+    <t>MARIA DANIELA</t>
+  </si>
+  <si>
+    <t>BORGES DELGADO</t>
+  </si>
+  <si>
+    <t>MARIANGEL</t>
+  </si>
+  <si>
+    <t>GUEVARA MENDOZA</t>
+  </si>
+  <si>
+    <t>OSNEIBE MAKEISI</t>
+  </si>
+  <si>
+    <t>AVILA CARDONA</t>
+  </si>
+  <si>
+    <t>ALIFER DE JESUS</t>
+  </si>
+  <si>
+    <t>PEREZ DELGADO</t>
+  </si>
+  <si>
+    <t>YOSMARY DEL VALLE</t>
+  </si>
+  <si>
+    <t>DIAZ VILLAROEL</t>
+  </si>
+  <si>
+    <t>KAHTERIN  DEL VALLE</t>
+  </si>
+  <si>
+    <t>FARIAS CASTILLO</t>
+  </si>
+  <si>
+    <t>STHEPHANY MISHELL</t>
+  </si>
+  <si>
+    <t>AGNESE ALCANTARA</t>
+  </si>
+  <si>
+    <t>JOSELYN ANDREINA</t>
+  </si>
+  <si>
+    <t>MEDINA MARCANO</t>
+  </si>
+  <si>
+    <t>YULEIDI DEL CARMEN</t>
+  </si>
+  <si>
+    <t>GALLEGOS ARCILES</t>
+  </si>
+  <si>
+    <t>KEINSLER ALEXANDER</t>
+  </si>
+  <si>
+    <t>CORDOVA PIÑANGO</t>
+  </si>
+  <si>
+    <t>IRIS MARLEY</t>
+  </si>
+  <si>
+    <t>JIMENEZ HERNANDEZ</t>
+  </si>
+  <si>
+    <t>YACNERY NAZARET</t>
+  </si>
+  <si>
+    <t>RIVAS ARAQUE</t>
+  </si>
+  <si>
+    <t>DARWIND NICOLAS</t>
+  </si>
+  <si>
+    <t>LOPEZ MANTILLA</t>
+  </si>
+  <si>
+    <t>GENESIS EURIMARIS</t>
+  </si>
+  <si>
+    <t>MUÑOZ RINCON</t>
+  </si>
+  <si>
+    <t>MANUEL ABRAHAM</t>
+  </si>
+  <si>
+    <t>BARRIOS APONTE</t>
+  </si>
+  <si>
+    <t>VICENTE ALEJANDRO</t>
+  </si>
+  <si>
+    <t>ISMARIEL PAOLA</t>
+  </si>
+  <si>
+    <t>FRANCO TINEO</t>
+  </si>
+  <si>
+    <t>JOSÉ ALEJANDRO</t>
+  </si>
+  <si>
+    <t>MORENO MAICABARE</t>
+  </si>
+  <si>
+    <t>ROMERO HERNANDEZ</t>
+  </si>
+  <si>
+    <t>JUAN MIGUEL</t>
+  </si>
+  <si>
+    <t>DEILYMAR ANGELICA</t>
+  </si>
+  <si>
+    <t>LABRADOR COELLO</t>
+  </si>
+  <si>
+    <t>JAIDERLIN VANESSA</t>
+  </si>
+  <si>
+    <t>FLORES FLORES</t>
+  </si>
+  <si>
+    <t>PAOLA VANESA</t>
+  </si>
+  <si>
+    <t>FLORES COLON</t>
+  </si>
+  <si>
+    <t>RAMIREZ MEDINA</t>
+  </si>
+  <si>
+    <t>ALFREDO JOSE</t>
+  </si>
+  <si>
+    <t>RONDON EURRESTA</t>
+  </si>
+  <si>
+    <t>KEIBEN JOSE</t>
+  </si>
+  <si>
+    <t>CASTELLANOS CALDERON</t>
+  </si>
+  <si>
+    <t>HILARY GISEL</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ NAVARRO</t>
+  </si>
+  <si>
+    <t>HIRDANYS MARGARETH</t>
+  </si>
+  <si>
+    <t>FERNANDEZ CHIRINOS</t>
+  </si>
+  <si>
+    <t>BERTHA JISSETH</t>
+  </si>
+  <si>
+    <t>MORENO BARRIENTOS</t>
+  </si>
+  <si>
+    <t>HECXELAY YOELY</t>
+  </si>
+  <si>
+    <t>INAGAS CHINCHILLA</t>
+  </si>
+  <si>
+    <t>ORIANA COROMOTO</t>
+  </si>
+  <si>
+    <t>PEREIRA AVENDAÑO</t>
+  </si>
+  <si>
+    <t>BARBARA GINESKA</t>
+  </si>
+  <si>
+    <t>DAVILA MARCANO</t>
+  </si>
+  <si>
+    <t>CALVELIS DE JESUS</t>
+  </si>
+  <si>
+    <t>EURRESTRA RIVERO</t>
+  </si>
+  <si>
+    <t>RAINER JOSE</t>
+  </si>
+  <si>
+    <t>MORENO MORENO</t>
+  </si>
+  <si>
+    <t>NAVIL RAFAEL</t>
+  </si>
+  <si>
+    <t>MENDEZ JIMENEZ</t>
+  </si>
+  <si>
+    <t>ZAMBRANO CAMACHO</t>
+  </si>
+  <si>
+    <t>DAVID RICARDO</t>
+  </si>
+  <si>
+    <t>BERNAL GARCIA</t>
+  </si>
+  <si>
+    <t>NANCY  VICTORIA</t>
+  </si>
+  <si>
+    <t>REYES CADENA</t>
+  </si>
+  <si>
+    <t>ELIZABETH COROMOTO</t>
+  </si>
+  <si>
+    <t>CORDOVA GUZMAN</t>
+  </si>
+  <si>
+    <t>DUNIA COROMOTO</t>
+  </si>
+  <si>
+    <t>YEGUEZ</t>
+  </si>
+  <si>
+    <t>WILMA SIMEON</t>
+  </si>
+  <si>
+    <t>YNFANTE RIVERO</t>
+  </si>
+  <si>
+    <t>FLORENTINO</t>
+  </si>
+  <si>
+    <t>CASTRO DE CHACON</t>
+  </si>
+  <si>
+    <t>NORVELIS COROMOTO</t>
+  </si>
+  <si>
+    <t>JAIMES GONZALEZ</t>
+  </si>
+  <si>
+    <t>ODALIS LOURDES</t>
+  </si>
+  <si>
+    <t>CALDERON MACHADO</t>
+  </si>
+  <si>
+    <t>MARIA INES</t>
+  </si>
+  <si>
+    <t>BELKIS YOLANDA</t>
+  </si>
+  <si>
+    <t>MANTILLA</t>
+  </si>
+  <si>
+    <t>YONELY COROMOTO</t>
+  </si>
+  <si>
+    <t>SPOSITO</t>
+  </si>
+  <si>
+    <t>EFRAIN</t>
+  </si>
+  <si>
+    <t>TORRES ACOSTA</t>
+  </si>
+  <si>
+    <t>PACHECO ALVAREZ</t>
+  </si>
+  <si>
+    <t>DELGADO R.</t>
+  </si>
+  <si>
+    <t>GLADIS JOSEFINA</t>
+  </si>
+  <si>
+    <t>BRUGUERA FIGUEROA</t>
+  </si>
+  <si>
+    <t>INGRID MARIANELA</t>
+  </si>
+  <si>
+    <t>CARMEN BALBINA</t>
+  </si>
+  <si>
+    <t>DÍAZ RODRÍGUEZ</t>
+  </si>
+  <si>
+    <t>MARRERO MUÑOZ</t>
+  </si>
+  <si>
+    <t>CARLOS RAFAEL</t>
+  </si>
+  <si>
+    <t>MONACO DI MASCIO</t>
+  </si>
+  <si>
+    <t>ROSANNA</t>
+  </si>
+  <si>
+    <t>HERNANDEZ ORTIZ</t>
+  </si>
+  <si>
+    <t>HUGO ALBERTO</t>
+  </si>
+  <si>
+    <t>BLANCA</t>
+  </si>
+  <si>
+    <t>ANTONIO DOMINGO</t>
+  </si>
+  <si>
+    <t>PEREZ COLINA</t>
+  </si>
+  <si>
+    <t>ROBIN GERONIMO</t>
+  </si>
+  <si>
+    <t>MONTOYA GOMEZ</t>
+  </si>
+  <si>
+    <t>NANCY CLARISA</t>
+  </si>
+  <si>
+    <t>LUGO JOHN</t>
+  </si>
+  <si>
+    <t>CARMEN DARIA</t>
+  </si>
+  <si>
+    <t>HERNANDEZ ROMERO</t>
+  </si>
+  <si>
+    <t>FLOR MARIA</t>
+  </si>
+  <si>
+    <t>CARRASQUEL MENA</t>
+  </si>
+  <si>
+    <t>CARMEN KATIUSCKA</t>
+  </si>
+  <si>
+    <t>FERNANDEZ LIENDO</t>
+  </si>
+  <si>
+    <t>NELSON RAFAEL</t>
   </si>
 </sst>
 </file>
@@ -6777,38 +7785,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6821,22 +7808,51 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -6853,30 +7869,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -6891,10 +7921,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6902,43 +7940,6 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -6951,7 +7952,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6963,7 +8054,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6975,7 +8066,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6987,67 +8102,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7059,79 +8132,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7164,72 +8165,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7252,156 +8188,221 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7727,10 +8728,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1306"/>
+  <dimension ref="A1:D1499"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A1335" workbookViewId="0">
+      <selection activeCell="A1304" sqref="A1304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="3"/>
@@ -26025,6 +27026,2708 @@
         <v>2251</v>
       </c>
     </row>
+    <row r="1307" spans="1:4">
+      <c r="A1307" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1307" s="1">
+        <v>10116448</v>
+      </c>
+      <c r="C1307" s="1" t="s">
+        <v>2253</v>
+      </c>
+      <c r="D1307" s="1" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:4">
+      <c r="A1308" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1308" s="1">
+        <v>10274289</v>
+      </c>
+      <c r="C1308" s="1" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D1308" s="1" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:4">
+      <c r="A1309" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1309" s="1">
+        <v>10350299</v>
+      </c>
+      <c r="C1309" s="1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D1309" s="1" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:4">
+      <c r="A1310" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1310" s="1">
+        <v>10353023</v>
+      </c>
+      <c r="C1310" s="1" t="s">
+        <v>2258</v>
+      </c>
+      <c r="D1310" s="1" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:4">
+      <c r="A1311" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1311" s="1">
+        <v>10378533</v>
+      </c>
+      <c r="C1311" s="1" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D1311" s="1" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:4">
+      <c r="A1312" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1312" s="1">
+        <v>10382279</v>
+      </c>
+      <c r="C1312" s="1" t="s">
+        <v>2261</v>
+      </c>
+      <c r="D1312" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:4">
+      <c r="A1313" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1313" s="1">
+        <v>10497243</v>
+      </c>
+      <c r="C1313" s="1" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D1313" s="1" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:4">
+      <c r="A1314" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1314" s="1">
+        <v>10504662</v>
+      </c>
+      <c r="C1314" s="1" t="s">
+        <v>2264</v>
+      </c>
+      <c r="D1314" s="1" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:4">
+      <c r="A1315" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1315" s="1">
+        <v>10524590</v>
+      </c>
+      <c r="C1315" s="1" t="s">
+        <v>2265</v>
+      </c>
+      <c r="D1315" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:4">
+      <c r="A1316" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1316" s="1">
+        <v>10536217</v>
+      </c>
+      <c r="C1316" s="1" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D1316" s="1" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:4">
+      <c r="A1317" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1317" s="1">
+        <v>10540514</v>
+      </c>
+      <c r="C1317" s="1" t="s">
+        <v>2268</v>
+      </c>
+      <c r="D1317" s="1" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:4">
+      <c r="A1318" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1318" s="1">
+        <v>10872142</v>
+      </c>
+      <c r="C1318" s="1" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D1318" s="1" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:4">
+      <c r="A1319" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1319" s="1">
+        <v>11312652</v>
+      </c>
+      <c r="C1319" s="1" t="s">
+        <v>2272</v>
+      </c>
+      <c r="D1319" s="1" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:4">
+      <c r="A1320" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1320" s="1">
+        <v>11529922</v>
+      </c>
+      <c r="C1320" s="1" t="s">
+        <v>2274</v>
+      </c>
+      <c r="D1320" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:4">
+      <c r="A1321" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1321" s="1">
+        <v>11557169</v>
+      </c>
+      <c r="C1321" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="D1321" s="1" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:4">
+      <c r="A1322" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1322" s="1">
+        <v>11560590</v>
+      </c>
+      <c r="C1322" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1322" s="1" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:4">
+      <c r="A1323" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1323" s="1">
+        <v>11602032</v>
+      </c>
+      <c r="C1323" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D1323" s="1" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:4">
+      <c r="A1324" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1324" s="1">
+        <v>11640949</v>
+      </c>
+      <c r="C1324" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="D1324" s="1" t="s">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:4">
+      <c r="A1325" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1325" s="1">
+        <v>11671858</v>
+      </c>
+      <c r="C1325" s="1" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D1325" s="1" t="s">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:4">
+      <c r="A1326" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1326" s="1">
+        <v>11686521</v>
+      </c>
+      <c r="C1326" s="1" t="s">
+        <v>2283</v>
+      </c>
+      <c r="D1326" s="1" t="s">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:4">
+      <c r="A1327" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1327" s="1">
+        <v>12059699</v>
+      </c>
+      <c r="C1327" s="1" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D1327" s="1" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:4">
+      <c r="A1328" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1328" s="1">
+        <v>12609498</v>
+      </c>
+      <c r="C1328" s="1" t="s">
+        <v>2285</v>
+      </c>
+      <c r="D1328" s="1" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:4">
+      <c r="A1329" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1329" s="1">
+        <v>12616960</v>
+      </c>
+      <c r="C1329" s="1" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D1329" s="1" t="s">
+        <v>2288</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:4">
+      <c r="A1330" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1330" s="1">
+        <v>12761698</v>
+      </c>
+      <c r="C1330" s="1" t="s">
+        <v>2289</v>
+      </c>
+      <c r="D1330" s="1" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:4">
+      <c r="A1331" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1331" s="1">
+        <v>12781596</v>
+      </c>
+      <c r="C1331" s="1" t="s">
+        <v>2291</v>
+      </c>
+      <c r="D1331" s="1" t="s">
+        <v>2292</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:4">
+      <c r="A1332" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1332" s="1">
+        <v>12832429</v>
+      </c>
+      <c r="C1332" s="1" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D1332" s="1" t="s">
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:4">
+      <c r="A1333" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1333" s="1">
+        <v>12910594</v>
+      </c>
+      <c r="C1333" s="1" t="s">
+        <v>2295</v>
+      </c>
+      <c r="D1333" s="1" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:4">
+      <c r="A1334" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1334" s="1">
+        <v>12927356</v>
+      </c>
+      <c r="C1334" s="1" t="s">
+        <v>2296</v>
+      </c>
+      <c r="D1334" s="1" t="s">
+        <v>2297</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:4">
+      <c r="A1335" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1335" s="1">
+        <v>12929373</v>
+      </c>
+      <c r="C1335" s="1" t="s">
+        <v>2298</v>
+      </c>
+      <c r="D1335" s="1" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:4">
+      <c r="A1336" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1336" s="1">
+        <v>13132613</v>
+      </c>
+      <c r="C1336" s="1" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D1336" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:4">
+      <c r="A1337" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1337" s="1">
+        <v>13133617</v>
+      </c>
+      <c r="C1337" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D1337" s="1" t="s">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:4">
+      <c r="A1338" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1338" s="1">
+        <v>13319726</v>
+      </c>
+      <c r="C1338" s="1" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D1338" s="1" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:4">
+      <c r="A1339" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1339" s="1">
+        <v>13432928</v>
+      </c>
+      <c r="C1339" s="1" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D1339" s="1" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:4">
+      <c r="A1340" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1340" s="1">
+        <v>13457501</v>
+      </c>
+      <c r="C1340" s="1" t="s">
+        <v>2306</v>
+      </c>
+      <c r="D1340" s="1" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:4">
+      <c r="A1341" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1341" s="1">
+        <v>13511213</v>
+      </c>
+      <c r="C1341" s="1" t="s">
+        <v>2308</v>
+      </c>
+      <c r="D1341" s="1" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:4">
+      <c r="A1342" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1342" s="1">
+        <v>13534113</v>
+      </c>
+      <c r="C1342" s="1" t="s">
+        <v>2310</v>
+      </c>
+      <c r="D1342" s="1" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:4">
+      <c r="A1343" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1343" s="1">
+        <v>13557983</v>
+      </c>
+      <c r="C1343" s="1" t="s">
+        <v>2312</v>
+      </c>
+      <c r="D1343" s="1" t="s">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:4">
+      <c r="A1344" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1344" s="1">
+        <v>13568697</v>
+      </c>
+      <c r="C1344" s="1" t="s">
+        <v>2314</v>
+      </c>
+      <c r="D1344" s="1" t="s">
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:4">
+      <c r="A1345" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1345" s="1">
+        <v>13721439</v>
+      </c>
+      <c r="C1345" s="1" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1345" s="1" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:4">
+      <c r="A1346" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1346" s="1">
+        <v>13780014</v>
+      </c>
+      <c r="C1346" s="1" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1346" s="1" t="s">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:4">
+      <c r="A1347" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1347" s="1">
+        <v>13870903</v>
+      </c>
+      <c r="C1347" s="1" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D1347" s="1" t="s">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:4">
+      <c r="A1348" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1348" s="1">
+        <v>13872371</v>
+      </c>
+      <c r="C1348" s="1" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D1348" s="1" t="s">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:4">
+      <c r="A1349" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1349" s="1">
+        <v>13884700</v>
+      </c>
+      <c r="C1349" s="1" t="s">
+        <v>2324</v>
+      </c>
+      <c r="D1349" s="1" t="s">
+        <v>2325</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:4">
+      <c r="A1350" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1350" s="1">
+        <v>13904616</v>
+      </c>
+      <c r="C1350" s="1" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D1350" s="1" t="s">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:4">
+      <c r="A1351" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1351" s="1">
+        <v>13951090</v>
+      </c>
+      <c r="C1351" s="1" t="s">
+        <v>2328</v>
+      </c>
+      <c r="D1351" s="1" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:4">
+      <c r="A1352" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1352" s="1">
+        <v>13978290</v>
+      </c>
+      <c r="C1352" s="1" t="s">
+        <v>2330</v>
+      </c>
+      <c r="D1352" s="1" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:4">
+      <c r="A1353" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1353" s="1">
+        <v>14000246</v>
+      </c>
+      <c r="C1353" s="1" t="s">
+        <v>2332</v>
+      </c>
+      <c r="D1353" s="1" t="s">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:4">
+      <c r="A1354" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1354" s="1">
+        <v>14184125</v>
+      </c>
+      <c r="C1354" s="1" t="s">
+        <v>2334</v>
+      </c>
+      <c r="D1354" s="1" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:4">
+      <c r="A1355" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1355" s="1">
+        <v>14241674</v>
+      </c>
+      <c r="C1355" s="1" t="s">
+        <v>2336</v>
+      </c>
+      <c r="D1355" s="1" t="s">
+        <v>2337</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:4">
+      <c r="A1356" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1356" s="1">
+        <v>14314690</v>
+      </c>
+      <c r="C1356" s="1" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D1356" s="1" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:4">
+      <c r="A1357" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1357" s="1">
+        <v>14360705</v>
+      </c>
+      <c r="C1357" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D1357" s="1" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:4">
+      <c r="A1358" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1358" s="1">
+        <v>14412299</v>
+      </c>
+      <c r="C1358" s="1" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D1358" s="1" t="s">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:4">
+      <c r="A1359" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1359" s="1">
+        <v>14453601</v>
+      </c>
+      <c r="C1359" s="1" t="s">
+        <v>2324</v>
+      </c>
+      <c r="D1359" s="1" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:4">
+      <c r="A1360" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1360" s="1">
+        <v>14656911</v>
+      </c>
+      <c r="C1360" s="1" t="s">
+        <v>2342</v>
+      </c>
+      <c r="D1360" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:4">
+      <c r="A1361" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1361" s="1">
+        <v>14788920</v>
+      </c>
+      <c r="C1361" s="1" t="s">
+        <v>2343</v>
+      </c>
+      <c r="D1361" s="1" t="s">
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:4">
+      <c r="A1362" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1362" s="1">
+        <v>14965562</v>
+      </c>
+      <c r="C1362" s="1" t="s">
+        <v>2345</v>
+      </c>
+      <c r="D1362" s="1" t="s">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:4">
+      <c r="A1363" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1363" s="1">
+        <v>14988835</v>
+      </c>
+      <c r="C1363" s="1" t="s">
+        <v>2347</v>
+      </c>
+      <c r="D1363" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:4">
+      <c r="A1364" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1364" s="1">
+        <v>15040918</v>
+      </c>
+      <c r="C1364" s="1" t="s">
+        <v>2348</v>
+      </c>
+      <c r="D1364" s="1" t="s">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:4">
+      <c r="A1365" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1365" s="1">
+        <v>15106422</v>
+      </c>
+      <c r="C1365" s="1" t="s">
+        <v>2350</v>
+      </c>
+      <c r="D1365" s="1" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:4">
+      <c r="A1366" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1366" s="1">
+        <v>15122600</v>
+      </c>
+      <c r="C1366" s="1" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D1366" s="1" t="s">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:4">
+      <c r="A1367" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1367" s="1">
+        <v>15324225</v>
+      </c>
+      <c r="C1367" s="1" t="s">
+        <v>2354</v>
+      </c>
+      <c r="D1367" s="1" t="s">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:4">
+      <c r="A1368" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1368" s="1">
+        <v>15337357</v>
+      </c>
+      <c r="C1368" s="1" t="s">
+        <v>2356</v>
+      </c>
+      <c r="D1368" s="1" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:4">
+      <c r="A1369" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1369" s="1">
+        <v>15487226</v>
+      </c>
+      <c r="C1369" s="1" t="s">
+        <v>2358</v>
+      </c>
+      <c r="D1369" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:4">
+      <c r="A1370" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1370" s="1">
+        <v>15505372</v>
+      </c>
+      <c r="C1370" s="1" t="s">
+        <v>2359</v>
+      </c>
+      <c r="D1370" s="1" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:4">
+      <c r="A1371" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1371" s="1">
+        <v>15507268</v>
+      </c>
+      <c r="C1371" s="1" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D1371" s="1" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:4">
+      <c r="A1372" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1372" s="1">
+        <v>15674054</v>
+      </c>
+      <c r="C1372" s="1" t="s">
+        <v>2363</v>
+      </c>
+      <c r="D1372" s="1" t="s">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:4">
+      <c r="A1373" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1373" s="1">
+        <v>15724821</v>
+      </c>
+      <c r="C1373" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="D1373" s="1" t="s">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:4">
+      <c r="A1374" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1374" s="1">
+        <v>15844746</v>
+      </c>
+      <c r="C1374" s="1" t="s">
+        <v>2367</v>
+      </c>
+      <c r="D1374" s="1" t="s">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:4">
+      <c r="A1375" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1375" s="1">
+        <v>16023041</v>
+      </c>
+      <c r="C1375" s="1" t="s">
+        <v>2369</v>
+      </c>
+      <c r="D1375" s="1" t="s">
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:4">
+      <c r="A1376" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1376" s="1">
+        <v>16056002</v>
+      </c>
+      <c r="C1376" s="1" t="s">
+        <v>2370</v>
+      </c>
+      <c r="D1376" s="1" t="s">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:4">
+      <c r="A1377" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1377" s="1">
+        <v>16087896</v>
+      </c>
+      <c r="C1377" s="1" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D1377" s="1" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:4">
+      <c r="A1378" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1378" s="1">
+        <v>16089888</v>
+      </c>
+      <c r="C1378" s="1" t="s">
+        <v>2374</v>
+      </c>
+      <c r="D1378" s="1" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:4">
+      <c r="A1379" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1379" s="1">
+        <v>16263914</v>
+      </c>
+      <c r="C1379" s="1" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D1379" s="1" t="s">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:4">
+      <c r="A1380" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1380" s="1">
+        <v>16343163</v>
+      </c>
+      <c r="C1380" s="1" t="s">
+        <v>2378</v>
+      </c>
+      <c r="D1380" s="1" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:4">
+      <c r="A1381" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1381" s="1">
+        <v>16405257</v>
+      </c>
+      <c r="C1381" s="1" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D1381" s="1" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:4">
+      <c r="A1382" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1382" s="1">
+        <v>16451259</v>
+      </c>
+      <c r="C1382" s="1" t="s">
+        <v>2382</v>
+      </c>
+      <c r="D1382" s="1" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:4">
+      <c r="A1383" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1383" s="1">
+        <v>16473560</v>
+      </c>
+      <c r="C1383" s="1" t="s">
+        <v>2310</v>
+      </c>
+      <c r="D1383" s="1" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:4">
+      <c r="A1384" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1384" s="1">
+        <v>16544622</v>
+      </c>
+      <c r="C1384" s="1" t="s">
+        <v>2385</v>
+      </c>
+      <c r="D1384" s="1" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:4">
+      <c r="A1385" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1385" s="1">
+        <v>16577477</v>
+      </c>
+      <c r="C1385" s="1" t="s">
+        <v>2387</v>
+      </c>
+      <c r="D1385" s="1" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:4">
+      <c r="A1386" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1386" s="1">
+        <v>16683605</v>
+      </c>
+      <c r="C1386" s="1" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D1386" s="1" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:4">
+      <c r="A1387" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1387" s="1">
+        <v>16766028</v>
+      </c>
+      <c r="C1387" s="1" t="s">
+        <v>2390</v>
+      </c>
+      <c r="D1387" s="1" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:4">
+      <c r="A1388" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1388" s="1">
+        <v>16778171</v>
+      </c>
+      <c r="C1388" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1388" s="1" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:4">
+      <c r="A1389" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1389" s="1">
+        <v>16903680</v>
+      </c>
+      <c r="C1389" s="1" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D1389" s="1" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:4">
+      <c r="A1390" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1390" s="1">
+        <v>16904729</v>
+      </c>
+      <c r="C1390" s="1" t="s">
+        <v>2394</v>
+      </c>
+      <c r="D1390" s="1" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:4">
+      <c r="A1391" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1391" s="1">
+        <v>17311810</v>
+      </c>
+      <c r="C1391" s="1" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D1391" s="1" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:4">
+      <c r="A1392" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1392" s="1">
+        <v>17390236</v>
+      </c>
+      <c r="C1392" s="1" t="s">
+        <v>2398</v>
+      </c>
+      <c r="D1392" s="1" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:4">
+      <c r="A1393" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1393" s="1">
+        <v>17406288</v>
+      </c>
+      <c r="C1393" s="1" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D1393" s="1" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:4">
+      <c r="A1394" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1394" s="1">
+        <v>17574404</v>
+      </c>
+      <c r="C1394" s="1" t="s">
+        <v>2402</v>
+      </c>
+      <c r="D1394" s="1" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:4">
+      <c r="A1395" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1395" s="1">
+        <v>17595452</v>
+      </c>
+      <c r="C1395" s="1" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D1395" s="1" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:4">
+      <c r="A1396" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1396" s="1">
+        <v>17677707</v>
+      </c>
+      <c r="C1396" s="1" t="s">
+        <v>2406</v>
+      </c>
+      <c r="D1396" s="1" t="s">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:4">
+      <c r="A1397" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1397" s="1">
+        <v>17806509</v>
+      </c>
+      <c r="C1397" s="1" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D1397" s="1" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:4">
+      <c r="A1398" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1398" s="1">
+        <v>17974177</v>
+      </c>
+      <c r="C1398" s="1" t="s">
+        <v>2410</v>
+      </c>
+      <c r="D1398" s="1" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:4">
+      <c r="A1399" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1399" s="1">
+        <v>17977211</v>
+      </c>
+      <c r="C1399" s="1" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D1399" s="1" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:4">
+      <c r="A1400" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1400" s="1">
+        <v>17982460</v>
+      </c>
+      <c r="C1400" s="1" t="s">
+        <v>2414</v>
+      </c>
+      <c r="D1400" s="1" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:4">
+      <c r="A1401" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1401" s="1">
+        <v>18039621</v>
+      </c>
+      <c r="C1401" s="1" t="s">
+        <v>2416</v>
+      </c>
+      <c r="D1401" s="1" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:4">
+      <c r="A1402" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1402" s="1">
+        <v>18164163</v>
+      </c>
+      <c r="C1402" s="1" t="s">
+        <v>2418</v>
+      </c>
+      <c r="D1402" s="1" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:4">
+      <c r="A1403" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1403" s="1">
+        <v>18525992</v>
+      </c>
+      <c r="C1403" s="1" t="s">
+        <v>2420</v>
+      </c>
+      <c r="D1403" s="1" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:4">
+      <c r="A1404" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1404" s="1">
+        <v>18721243</v>
+      </c>
+      <c r="C1404" s="1" t="s">
+        <v>1897</v>
+      </c>
+      <c r="D1404" s="1" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:4">
+      <c r="A1405" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1405" s="1">
+        <v>18818541</v>
+      </c>
+      <c r="C1405" s="1" t="s">
+        <v>2422</v>
+      </c>
+      <c r="D1405" s="1" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:4">
+      <c r="A1406" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1406" s="1">
+        <v>18875503</v>
+      </c>
+      <c r="C1406" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="D1406" s="1" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:4">
+      <c r="A1407" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1407" s="1">
+        <v>18899906</v>
+      </c>
+      <c r="C1407" s="1" t="s">
+        <v>2426</v>
+      </c>
+      <c r="D1407" s="1" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:4">
+      <c r="A1408" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1408" s="1">
+        <v>18914078</v>
+      </c>
+      <c r="C1408" s="1" t="s">
+        <v>2428</v>
+      </c>
+      <c r="D1408" s="1" t="s">
+        <v>2429</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:4">
+      <c r="A1409" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1409" s="1">
+        <v>18934422</v>
+      </c>
+      <c r="C1409" s="1" t="s">
+        <v>2430</v>
+      </c>
+      <c r="D1409" s="1" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:4">
+      <c r="A1410" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1410" s="1">
+        <v>18975820</v>
+      </c>
+      <c r="C1410" s="1" t="s">
+        <v>2432</v>
+      </c>
+      <c r="D1410" s="1" t="s">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:4">
+      <c r="A1411" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1411" s="1">
+        <v>18976811</v>
+      </c>
+      <c r="C1411" s="1" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1411" s="1" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:4">
+      <c r="A1412" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1412" s="1">
+        <v>18982449</v>
+      </c>
+      <c r="C1412" s="1" t="s">
+        <v>2435</v>
+      </c>
+      <c r="D1412" s="1" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:4">
+      <c r="A1413" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1413" s="1">
+        <v>19224741</v>
+      </c>
+      <c r="C1413" s="1" t="s">
+        <v>2436</v>
+      </c>
+      <c r="D1413" s="1" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:4">
+      <c r="A1414" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1414" s="1">
+        <v>19293863</v>
+      </c>
+      <c r="C1414" s="1" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D1414" s="1" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:4">
+      <c r="A1415" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1415" s="1">
+        <v>19334879</v>
+      </c>
+      <c r="C1415" s="1" t="s">
+        <v>2440</v>
+      </c>
+      <c r="D1415" s="1" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:4">
+      <c r="A1416" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1416" s="1">
+        <v>19477759</v>
+      </c>
+      <c r="C1416" s="1" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D1416" s="1" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:4">
+      <c r="A1417" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1417" s="1">
+        <v>19581326</v>
+      </c>
+      <c r="C1417" s="1" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D1417" s="1" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:4">
+      <c r="A1418" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1418" s="1">
+        <v>19653637</v>
+      </c>
+      <c r="C1418" s="1" t="s">
+        <v>2446</v>
+      </c>
+      <c r="D1418" s="1" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:4">
+      <c r="A1419" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1419" s="1">
+        <v>19933797</v>
+      </c>
+      <c r="C1419" s="1" t="s">
+        <v>2447</v>
+      </c>
+      <c r="D1419" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:4">
+      <c r="A1420" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1420" s="1">
+        <v>19947984</v>
+      </c>
+      <c r="C1420" s="1" t="s">
+        <v>2448</v>
+      </c>
+      <c r="D1420" s="1" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:4">
+      <c r="A1421" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1421" s="1">
+        <v>20033232</v>
+      </c>
+      <c r="C1421" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="D1421" s="1" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:4">
+      <c r="A1422" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1422" s="1">
+        <v>20129882</v>
+      </c>
+      <c r="C1422" s="1" t="s">
+        <v>2452</v>
+      </c>
+      <c r="D1422" s="1" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:4">
+      <c r="A1423" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1423" s="1">
+        <v>20130703</v>
+      </c>
+      <c r="C1423" s="1" t="s">
+        <v>2454</v>
+      </c>
+      <c r="D1423" s="1" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:4">
+      <c r="A1424" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1424" s="1">
+        <v>20132572</v>
+      </c>
+      <c r="C1424" s="1" t="s">
+        <v>2456</v>
+      </c>
+      <c r="D1424" s="1" t="s">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:4">
+      <c r="A1425" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1425" s="1">
+        <v>20211320</v>
+      </c>
+      <c r="C1425" s="1" t="s">
+        <v>2458</v>
+      </c>
+      <c r="D1425" s="1" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:4">
+      <c r="A1426" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1426" s="1">
+        <v>20221939</v>
+      </c>
+      <c r="C1426" s="1" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D1426" s="1" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:4">
+      <c r="A1427" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1427" s="1">
+        <v>20270646</v>
+      </c>
+      <c r="C1427" s="1" t="s">
+        <v>2461</v>
+      </c>
+      <c r="D1427" s="1" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:4">
+      <c r="A1428" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1428" s="1">
+        <v>20483362</v>
+      </c>
+      <c r="C1428" s="1" t="s">
+        <v>2463</v>
+      </c>
+      <c r="D1428" s="1" t="s">
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:4">
+      <c r="A1429" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1429" s="1">
+        <v>20593653</v>
+      </c>
+      <c r="C1429" s="1" t="s">
+        <v>2465</v>
+      </c>
+      <c r="D1429" s="1" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:4">
+      <c r="A1430" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1430" s="1">
+        <v>20639809</v>
+      </c>
+      <c r="C1430" s="1" t="s">
+        <v>2467</v>
+      </c>
+      <c r="D1430" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:4">
+      <c r="A1431" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1431" s="1">
+        <v>20654138</v>
+      </c>
+      <c r="C1431" s="1" t="s">
+        <v>2468</v>
+      </c>
+      <c r="D1431" s="1" t="s">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:4">
+      <c r="A1432" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1432" s="1">
+        <v>20673369</v>
+      </c>
+      <c r="C1432" s="1" t="s">
+        <v>2470</v>
+      </c>
+      <c r="D1432" s="1" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:4">
+      <c r="A1433" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1433" s="1">
+        <v>20791575</v>
+      </c>
+      <c r="C1433" s="1" t="s">
+        <v>2472</v>
+      </c>
+      <c r="D1433" s="1" t="s">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:4">
+      <c r="A1434" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1434" s="1">
+        <v>21072827</v>
+      </c>
+      <c r="C1434" s="1" t="s">
+        <v>2474</v>
+      </c>
+      <c r="D1434" s="1" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:4">
+      <c r="A1435" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1435" s="1">
+        <v>21176096</v>
+      </c>
+      <c r="C1435" s="1" t="s">
+        <v>2476</v>
+      </c>
+      <c r="D1435" s="1" t="s">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:4">
+      <c r="A1436" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1436" s="1">
+        <v>21193408</v>
+      </c>
+      <c r="C1436" s="1" t="s">
+        <v>2478</v>
+      </c>
+      <c r="D1436" s="1" t="s">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:4">
+      <c r="A1437" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1437" s="1">
+        <v>21193956</v>
+      </c>
+      <c r="C1437" s="1" t="s">
+        <v>2480</v>
+      </c>
+      <c r="D1437" s="1" t="s">
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:4">
+      <c r="A1438" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1438" s="1">
+        <v>21346651</v>
+      </c>
+      <c r="C1438" s="1" t="s">
+        <v>2482</v>
+      </c>
+      <c r="D1438" s="1" t="s">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:4">
+      <c r="A1439" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1439" s="1">
+        <v>21759418</v>
+      </c>
+      <c r="C1439" s="1" t="s">
+        <v>2484</v>
+      </c>
+      <c r="D1439" s="1" t="s">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:4">
+      <c r="A1440" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1440" s="1">
+        <v>22436005</v>
+      </c>
+      <c r="C1440" s="1" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D1440" s="1" t="s">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:4">
+      <c r="A1441" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1441" s="1">
+        <v>22447672</v>
+      </c>
+      <c r="C1441" s="1" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D1441" s="1" t="s">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:4">
+      <c r="A1442" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1442" s="1">
+        <v>22566461</v>
+      </c>
+      <c r="C1442" s="1" t="s">
+        <v>2490</v>
+      </c>
+      <c r="D1442" s="1" t="s">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:4">
+      <c r="A1443" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1443" s="1">
+        <v>22904493</v>
+      </c>
+      <c r="C1443" s="1" t="s">
+        <v>2492</v>
+      </c>
+      <c r="D1443" s="1" t="s">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:4">
+      <c r="A1444" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1444" s="1">
+        <v>23529477</v>
+      </c>
+      <c r="C1444" s="1" t="s">
+        <v>2494</v>
+      </c>
+      <c r="D1444" s="1" t="s">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:4">
+      <c r="A1445" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1445" s="1">
+        <v>23713130</v>
+      </c>
+      <c r="C1445" s="1" t="s">
+        <v>2496</v>
+      </c>
+      <c r="D1445" s="1" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:4">
+      <c r="A1446" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1446" s="1">
+        <v>23943246</v>
+      </c>
+      <c r="C1446" s="1" t="s">
+        <v>2498</v>
+      </c>
+      <c r="D1446" s="1" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:4">
+      <c r="A1447" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1447" s="1">
+        <v>24277925</v>
+      </c>
+      <c r="C1447" s="1" t="s">
+        <v>2500</v>
+      </c>
+      <c r="D1447" s="1" t="s">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:4">
+      <c r="A1448" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1448" s="1">
+        <v>24288691</v>
+      </c>
+      <c r="C1448" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="D1448" s="1" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:4">
+      <c r="A1449" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1449" s="1">
+        <v>24312360</v>
+      </c>
+      <c r="C1449" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D1449" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:4">
+      <c r="A1450" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1450" s="1">
+        <v>24625318</v>
+      </c>
+      <c r="C1450" s="1" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D1450" s="1" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:4">
+      <c r="A1451" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1451" s="1">
+        <v>24757274</v>
+      </c>
+      <c r="C1451" s="1" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D1451" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:4">
+      <c r="A1452" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1452" s="1">
+        <v>24895749</v>
+      </c>
+      <c r="C1452" s="1" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D1452" s="1" t="s">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:4">
+      <c r="A1453" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1453" s="1">
+        <v>24940686</v>
+      </c>
+      <c r="C1453" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1453" s="1" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:4">
+      <c r="A1454" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1454" s="1">
+        <v>25029177</v>
+      </c>
+      <c r="C1454" s="1" t="s">
+        <v>2509</v>
+      </c>
+      <c r="D1454" s="1" t="s">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:4">
+      <c r="A1455" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1455" s="1">
+        <v>25222996</v>
+      </c>
+      <c r="C1455" s="1" t="s">
+        <v>2511</v>
+      </c>
+      <c r="D1455" s="1" t="s">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:4">
+      <c r="A1456" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1456" s="1">
+        <v>25386863</v>
+      </c>
+      <c r="C1456" s="1" t="s">
+        <v>2513</v>
+      </c>
+      <c r="D1456" s="1" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:4">
+      <c r="A1457" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1457" s="1">
+        <v>25466184</v>
+      </c>
+      <c r="C1457" s="1" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D1457" s="1" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:4">
+      <c r="A1458" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1458" s="1">
+        <v>25872150</v>
+      </c>
+      <c r="C1458" s="1" t="s">
+        <v>2516</v>
+      </c>
+      <c r="D1458" s="1" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:4">
+      <c r="A1459" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1459" s="1">
+        <v>26114744</v>
+      </c>
+      <c r="C1459" s="1" t="s">
+        <v>2518</v>
+      </c>
+      <c r="D1459" s="1" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:4">
+      <c r="A1460" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1460" s="1">
+        <v>26600887</v>
+      </c>
+      <c r="C1460" s="1" t="s">
+        <v>2520</v>
+      </c>
+      <c r="D1460" s="1" t="s">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:4">
+      <c r="A1461" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1461" s="1">
+        <v>27020355</v>
+      </c>
+      <c r="C1461" s="1" t="s">
+        <v>2522</v>
+      </c>
+      <c r="D1461" s="1" t="s">
+        <v>2523</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:4">
+      <c r="A1462" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1462" s="1">
+        <v>27373268</v>
+      </c>
+      <c r="C1462" s="1" t="s">
+        <v>2524</v>
+      </c>
+      <c r="D1462" s="1" t="s">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:4">
+      <c r="A1463" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1463" s="1">
+        <v>27449688</v>
+      </c>
+      <c r="C1463" s="1" t="s">
+        <v>2526</v>
+      </c>
+      <c r="D1463" s="1" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:4">
+      <c r="A1464" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1464" s="1">
+        <v>27755986</v>
+      </c>
+      <c r="C1464" s="1" t="s">
+        <v>2528</v>
+      </c>
+      <c r="D1464" s="1" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:4">
+      <c r="A1465" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1465" s="1">
+        <v>28100760</v>
+      </c>
+      <c r="C1465" s="1" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D1465" s="1" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:4">
+      <c r="A1466" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1466" s="1">
+        <v>29533572</v>
+      </c>
+      <c r="C1466" s="1" t="s">
+        <v>2532</v>
+      </c>
+      <c r="D1466" s="1" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:4">
+      <c r="A1467" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1467" s="1">
+        <v>30032026</v>
+      </c>
+      <c r="C1467" s="1" t="s">
+        <v>2534</v>
+      </c>
+      <c r="D1467" s="1" t="s">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:4">
+      <c r="A1468" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1468" s="1">
+        <v>3721931</v>
+      </c>
+      <c r="C1468" s="1" t="s">
+        <v>2536</v>
+      </c>
+      <c r="D1468" s="1" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:4">
+      <c r="A1469" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1469" s="1">
+        <v>4682071</v>
+      </c>
+      <c r="C1469" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="D1469" s="1" t="s">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:4">
+      <c r="A1470" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1470" s="1">
+        <v>5301768</v>
+      </c>
+      <c r="C1470" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="D1470" s="1" t="s">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:4">
+      <c r="A1471" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1471" s="1">
+        <v>5466003</v>
+      </c>
+      <c r="C1471" s="1" t="s">
+        <v>2541</v>
+      </c>
+      <c r="D1471" s="1" t="s">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:4">
+      <c r="A1472" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1472" s="1">
+        <v>5565072</v>
+      </c>
+      <c r="C1472" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D1472" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:4">
+      <c r="A1473" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1473" s="1">
+        <v>5881379</v>
+      </c>
+      <c r="C1473" s="1" t="s">
+        <v>2543</v>
+      </c>
+      <c r="D1473" s="1" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:4">
+      <c r="A1474" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1474" s="1">
+        <v>5913952</v>
+      </c>
+      <c r="C1474" s="1" t="s">
+        <v>2545</v>
+      </c>
+      <c r="D1474" s="1" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:4">
+      <c r="A1475" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1475" s="1">
+        <v>6047444</v>
+      </c>
+      <c r="C1475" s="1" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D1475" s="1" t="s">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:4">
+      <c r="A1476" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1476" s="1">
+        <v>6059084</v>
+      </c>
+      <c r="C1476" s="1" t="s">
+        <v>2549</v>
+      </c>
+      <c r="D1476" s="1" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:4">
+      <c r="A1477" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1477" s="1">
+        <v>6176649</v>
+      </c>
+      <c r="C1477" s="1" t="s">
+        <v>2551</v>
+      </c>
+      <c r="D1477" s="1" t="s">
+        <v>2552</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:4">
+      <c r="A1478" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1478" s="1">
+        <v>6193109</v>
+      </c>
+      <c r="C1478" s="1" t="s">
+        <v>2553</v>
+      </c>
+      <c r="D1478" s="1" t="s">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:4">
+      <c r="A1479" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1479" s="1">
+        <v>6205095</v>
+      </c>
+      <c r="C1479" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1479" s="1" t="s">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:4">
+      <c r="A1480" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1480" s="1">
+        <v>6270747</v>
+      </c>
+      <c r="C1480" s="1" t="s">
+        <v>2556</v>
+      </c>
+      <c r="D1480" s="1" t="s">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:4">
+      <c r="A1481" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1481" s="1">
+        <v>6309119</v>
+      </c>
+      <c r="C1481" s="1" t="s">
+        <v>2558</v>
+      </c>
+      <c r="D1481" s="1" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:4">
+      <c r="A1482" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1482" s="1">
+        <v>6432551</v>
+      </c>
+      <c r="C1482" s="1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="D1482" s="1" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:4">
+      <c r="A1483" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1483" s="1">
+        <v>6435696</v>
+      </c>
+      <c r="C1483" s="1" t="s">
+        <v>2561</v>
+      </c>
+      <c r="D1483" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:4">
+      <c r="A1484" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1484" s="1">
+        <v>6450769</v>
+      </c>
+      <c r="C1484" s="1" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D1484" s="1" t="s">
+        <v>2563</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:4">
+      <c r="A1485" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1485" s="1">
+        <v>6475653</v>
+      </c>
+      <c r="C1485" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D1485" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:4">
+      <c r="A1486" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1486" s="1">
+        <v>6516225</v>
+      </c>
+      <c r="C1486" s="1" t="s">
+        <v>2564</v>
+      </c>
+      <c r="D1486" s="1" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:4">
+      <c r="A1487" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1487" s="1">
+        <v>6730884</v>
+      </c>
+      <c r="C1487" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D1487" s="1" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:4">
+      <c r="A1488" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1488" s="1">
+        <v>7233228</v>
+      </c>
+      <c r="C1488" s="1" t="s">
+        <v>2567</v>
+      </c>
+      <c r="D1488" s="1" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:4">
+      <c r="A1489" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1489" s="1">
+        <v>7920566</v>
+      </c>
+      <c r="C1489" s="1" t="s">
+        <v>2568</v>
+      </c>
+      <c r="D1489" s="1" t="s">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:4">
+      <c r="A1490" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1490" s="1">
+        <v>7955454</v>
+      </c>
+      <c r="C1490" s="1" t="s">
+        <v>2570</v>
+      </c>
+      <c r="D1490" s="1" t="s">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:4">
+      <c r="A1491" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1491" s="1">
+        <v>83036958</v>
+      </c>
+      <c r="C1491" s="1" t="s">
+        <v>2572</v>
+      </c>
+      <c r="D1491" s="1" t="s">
+        <v>2573</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:4">
+      <c r="A1492" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1492" s="1">
+        <v>8371271</v>
+      </c>
+      <c r="C1492" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="D1492" s="1" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:4">
+      <c r="A1493" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1493" s="1">
+        <v>8634386</v>
+      </c>
+      <c r="C1493" s="1" t="s">
+        <v>2576</v>
+      </c>
+      <c r="D1493" s="1" t="s">
+        <v>2577</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:4">
+      <c r="A1494" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1494" s="1">
+        <v>8691690</v>
+      </c>
+      <c r="C1494" s="1" t="s">
+        <v>2578</v>
+      </c>
+      <c r="D1494" s="1" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:4">
+      <c r="A1495" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1495" s="1">
+        <v>8758082</v>
+      </c>
+      <c r="C1495" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D1495" s="1" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:4">
+      <c r="A1496" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1496" s="1">
+        <v>8761898</v>
+      </c>
+      <c r="C1496" s="1" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D1496" s="1" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:4">
+      <c r="A1497" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1497" s="1">
+        <v>9388547</v>
+      </c>
+      <c r="C1497" s="1" t="s">
+        <v>2582</v>
+      </c>
+      <c r="D1497" s="1" t="s">
+        <v>2583</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:4">
+      <c r="A1498" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1498" s="1">
+        <v>9487130</v>
+      </c>
+      <c r="C1498" s="1" t="s">
+        <v>2584</v>
+      </c>
+      <c r="D1498" s="1" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:4">
+      <c r="A1499" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1499" s="1">
+        <v>9661808</v>
+      </c>
+      <c r="C1499" s="1" t="s">
+        <v>2586</v>
+      </c>
+      <c r="D1499" s="1" t="s">
+        <v>2587</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>